<commit_message>
Updating data dictionary with data types
</commit_message>
<xml_diff>
--- a/ppp-data-dictionary-umd.xlsx
+++ b/ppp-data-dictionary-umd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekwillis/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smussenden/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18CEA4E-D673-6E4C-A1DE-BD10EE5E8DB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968A734B-24C4-9041-BB9F-A677BAE5BF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{B3E6CDFA-0DAE-46C7-ADEA-1E35C19B6803}"/>
+    <workbookView xWindow="16520" yWindow="2400" windowWidth="24140" windowHeight="20060" xr2:uid="{B3E6CDFA-0DAE-46C7-ADEA-1E35C19B6803}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>Business Age Description</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Project County Name</t>
   </si>
   <si>
-    <t>NAICS 6 digit code</t>
-  </si>
-  <si>
     <t>Field Name</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
     <t>Undisbursed Amount</t>
   </si>
   <si>
-    <t>Rural or Urban Indicator (R/U)</t>
-  </si>
-  <si>
-    <t>Hubzone Indicator (Y/N)</t>
-  </si>
-  <si>
     <t>Project City</t>
   </si>
   <si>
@@ -240,9 +231,6 @@
   </si>
   <si>
     <t>Loan Maturity in Months</t>
-  </si>
-  <si>
-    <t>LMI Indicator (Y/N)</t>
   </si>
   <si>
     <t>Project Zip Code</t>
@@ -284,13 +272,37 @@
   </si>
   <si>
     <t>Forgiveness Paid Date</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>NAICS 6 digit code that defines the industry of the borrower. https://www.census.gov/naics/?58967?yearbck=2017</t>
+  </si>
+  <si>
+    <t>Rural or Urban Indicator (R/U) https://www.ers.usda.gov/data-products/rural-urban-continuum-codes/</t>
+  </si>
+  <si>
+    <t>Hubzone Indicator (Y/N) https://www.sba.gov/federal-contracting/contracting-assistance-programs/hubzone-program</t>
+  </si>
+  <si>
+    <t>LMI Indicator (Y/N) https://www.sba.gov/partners/sbics/operate-sbic</t>
+  </si>
+  <si>
+    <t>DataType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +314,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -353,6 +372,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2331749F-B552-4C82-BE83-FE3F9B17F32E}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -679,332 +699,455 @@
     <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="C39" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="C41" s="6" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>